<commit_message>
editar datos usuarios y tardanza justificada
</commit_message>
<xml_diff>
--- a/Registros/14-11-2025.xlsx
+++ b/Registros/14-11-2025.xlsx
@@ -4,24 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Docentes" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Tarde" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Mañana" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="Tarde" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
-  <si>
-    <t>REGISTRO DE ASISTENCIA - DOCENTES</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+  <si>
+    <t>REGISTRO DE ASISTENCIA - SEMIANUAL - TARDE</t>
   </si>
   <si>
     <t>N°</t>
   </si>
   <si>
-    <t>DOCENTE</t>
+    <t>ALUMNO</t>
   </si>
   <si>
     <t>TURNO</t>
@@ -33,47 +31,29 @@
     <t>VIERNES 14</t>
   </si>
   <si>
-    <t>ALIAGA PEREZ ALAN OSCAR</t>
-  </si>
-  <si>
-    <t/>
+    <t>ALIAGA URIONDO JHERSON LEONARDO</t>
+  </si>
+  <si>
+    <t>TARDE</t>
   </si>
   <si>
     <t>L, M, MI, J, V, S</t>
   </si>
   <si>
-    <t>08:54A.M.</t>
-  </si>
-  <si>
-    <t>REGISTRO DE ASISTENCIA - SEMIANUAL - TARDE</t>
-  </si>
-  <si>
-    <t>ALUMNO</t>
-  </si>
-  <si>
-    <t>ALIAGA URIONDO JHERSON LEONARDO</t>
-  </si>
-  <si>
-    <t>TARDE</t>
-  </si>
-  <si>
-    <t>08:55A.M.</t>
-  </si>
-  <si>
-    <t>REGISTRO DE ASISTENCIA - SEMIANUAL - MAÑANA</t>
+    <t>10:52P.M.</t>
   </si>
   <si>
     <t>URIONDO MANINI CARLA DAYDAMIA</t>
   </si>
   <si>
-    <t>MAÑANA</t>
+    <t>10:52P.M. (J)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -94,18 +74,14 @@
     </font>
     <font>
       <b/>
-      <color rgb="FF000000"/>
+      <color rgb="FF9C0006"/>
     </font>
     <font>
       <b/>
-      <color rgb="FF006100"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,27 +90,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF1F4E78"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF404040"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,13 +140,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -522,7 +482,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -575,68 +535,21 @@
         <v>9</v>
       </c>
     </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -646,68 +559,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>